<commit_message>
Consolidates non-text run tags.
git-svn-id: https://okapi.googlecode.com/svn/trunk@1902 0cd2bb99-014b-0410-b875-5d0485b745ed
</commit_message>
<xml_diff>
--- a/filters/net.sf.okapi.filters.openxml.tests/gold/Peeksample.xlsx
+++ b/filters/net.sf.okapi.filters.openxml.tests/gold/Peeksample.xlsx
@@ -15,8 +15,39 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10"><si><t>oremlay<w:br/>[MARKER_ISOLATED 0:]<w:br/></t></si><si><t>ipsumhay<w:br/>[MARKER_ISOLATED 0:]<w:br/></t></si><si><t>olorday<w:br/>[MARKER_ISOLATED 0:]<w:br/></t></si><si><t>itsay<w:br/>[MARKER_ISOLATED 0:]<w:br/></t></si><si><t>amethay<w:br/>[MARKER_ISOLATED 0:]<w:br/></t></si><si><t>onsectetuercay<w:br/>[MARKER_ISOLATED 0:]<w:br/></t></si><si><t>adipiscinghay<w:br/>[MARKER_ISOLATED 0:]<w:br/></t></si><si><t>elithay<w:br/>[MARKER_ISOLATED 0:]<w:br/></t></si><si><t>uncnay<w:br/>[MARKER_ISOLATED 0:]<w:br/></t></si><si><t>athay<w:br/>[MARKER_ISOLATED 0:]<w:br/></t></si></sst>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>oremlay</t>
+  </si>
+  <si>
+    <t>ipsumhay</t>
+  </si>
+  <si>
+    <t>olorday</t>
+  </si>
+  <si>
+    <t>itsay</t>
+  </si>
+  <si>
+    <t>amethay</t>
+  </si>
+  <si>
+    <t>onsectetuercay</t>
+  </si>
+  <si>
+    <t>adipiscinghay</t>
+  </si>
+  <si>
+    <t>elithay</t>
+  </si>
+  <si>
+    <t>uncnay</t>
+  </si>
+  <si>
+    <t>athay</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -344,8 +375,99 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"><dimension ref="A1:B10"/><sheetViews><sheetView tabSelected="1" workbookViewId="0"/></sheetViews><sheetFormatPr defaultRowHeight="15"/><sheetData><row r="1" spans="1:2"><c r="A1" t="s"><v>0<w:br/>[MARKER_ISOLATED 0:]<w:br/></v></c><c r="B1"><v>111<w:br/>[MARKER_ISOLATED 0:]<w:br/></v></c></row><row r="2" spans="1:2"><c r="A2" t="s"><v>1<w:br/>[MARKER_ISOLATED 0:]<w:br/></v></c><c r="B2"><v>222<w:br/>[MARKER_ISOLATED 0:]<w:br/></v></c></row><row r="3" spans="1:2"><c r="A3" t="s"><v>2<w:br/>[MARKER_ISOLATED 0:]<w:br/></v></c><c r="B3"><v>333<w:br/>[MARKER_ISOLATED 0:]<w:br/></v></c></row><row r="4" spans="1:2"><c r="A4" t="s"><v>3<w:br/>[MARKER_ISOLATED 0:]<w:br/></v></c><c r="B4"><v>444<w:br/>[MARKER_ISOLATED 0:]<w:br/></v></c></row><row r="5" spans="1:2"><c r="A5" t="s"><v>4<w:br/>[MARKER_ISOLATED 0:]<w:br/></v></c><c r="B5"><v>555<w:br/>[MARKER_ISOLATED 0:]<w:br/></v></c></row><row r="6" spans="1:2"><c r="A6" t="s"><v>5<w:br/>[MARKER_ISOLATED 0:]<w:br/></v></c><c r="B6"><v>666<w:br/>[MARKER_ISOLATED 0:]<w:br/></v></c></row><row r="7" spans="1:2"><c r="A7" t="s"><v>6<w:br/>[MARKER_ISOLATED 0:]<w:br/></v></c><c r="B7"><v>777<w:br/>[MARKER_ISOLATED 0:]<w:br/></v></c></row><row r="8" spans="1:2"><c r="A8" t="s"><v>7<w:br/>[MARKER_ISOLATED 0:]<w:br/></v></c><c r="B8"><v>888<w:br/>[MARKER_ISOLATED 0:]<w:br/></v></c></row><row r="9" spans="1:2"><c r="A9" t="s"><v>8<w:br/>[MARKER_ISOLATED 0:]<w:br/></v></c><c r="B9"><v>999<w:br/>[MARKER_ISOLATED 0:]<w:br/></v></c></row><row r="10" spans="1:2"><c r="A10" t="s"><v>9<w:br/>[MARKER_ISOLATED 0:]<w:br/></v></c><c r="B10"><f>SUM(B1:B9)</f><v>4995<w:br/>[MARKER_ISOLATED 0:]<w:br/></v></c></row></sheetData><pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/><pageSetup orientation="portrait" r:id="rId1"/></worksheet>
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f>SUM(B1:B9)</f>
+        <v>4995</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>